<commit_message>
Two testcases commit: TC3 & TC4
TC3: Verify landing Pages for various users
TC4: Verify error messages for these users
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/sauceDemoLoginTestData.xlsx
+++ b/src/test/resources/testdata/sauceDemoLoginTestData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Library\I - Jan - March Automation\LoginModulesAutomation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2545F0D-82CC-44FB-86C3-5EC02CD1823A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA863A04-EC52-482F-97C7-757AF3800F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verifyEmailFieldFormat" sheetId="1" r:id="rId1"/>
+    <sheet name="verifyLandingPages" sheetId="2" r:id="rId2"/>
+    <sheet name="verifyLandingPagesInvalidUser" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -43,16 +45,40 @@
   </si>
   <si>
     <t>nonsense</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>error_user</t>
+  </si>
+  <si>
+    <t>visual_user</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,8 +104,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,7 +389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -407,4 +434,106 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082BDED4-2B82-4B47-8A0B-A02EDF57EF93}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97DC781-F51F-4DE5-AD85-BEA3F457E766}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>